<commit_message>
changes on taxonomies for data to be suitable for documents
</commit_message>
<xml_diff>
--- a/data/excel/funders.xlsx
+++ b/data/excel/funders.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\taxonomie\současné_hotové\aktualne_pouzite_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moon.ntkcz.cz\petka\NUŠL\SW\INVENIO 3\taxonomie\současné_hotové\NR_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12630" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8328" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nr" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="344">
   <si>
     <t>code</t>
   </si>
@@ -485,15 +485,6 @@
     <t>GA UK</t>
   </si>
   <si>
-    <t>CEA</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>ESF</t>
   </si>
   <si>
@@ -1034,12 +1025,6 @@
     <t>Research funders</t>
   </si>
   <si>
-    <t>aliases_0</t>
-  </si>
-  <si>
-    <t>aliases_1</t>
-  </si>
-  <si>
     <t>CAS</t>
   </si>
   <si>
@@ -1064,13 +1049,16 @@
     <t>Technology Agency of the Czech Republic</t>
   </si>
   <si>
-    <t>relatedURI_DOI</t>
-  </si>
-  <si>
     <t>relatedURI_ROR</t>
   </si>
   <si>
-    <t>formerTitles_en_0</t>
+    <t>nonpreferredLabels_en_0</t>
+  </si>
+  <si>
+    <t>acronym</t>
+  </si>
+  <si>
+    <t>relatedURI_CrossrefFunderID</t>
   </si>
 </sst>
 </file>
@@ -1489,29 +1477,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="25.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
+    <col min="11" max="11" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75">
+    <row r="1" spans="1:12" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,9 +1518,8 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75">
+    </row>
+    <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1539,7 +1527,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1549,9 +1537,8 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75">
+    </row>
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1563,9 +1550,8 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75">
+    </row>
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1579,37 +1565,31 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>336</v>
+        <v>342</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1620,9 +1600,11 @@
         <v>135</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>336</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>332</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -1630,20 +1612,14 @@
       <c r="J6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="L6" t="s">
-        <v>153</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75">
+      <c r="K6" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1665,15 +1641,11 @@
         <v>75</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" t="s">
-        <v>153</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="18" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75">
+      <c r="L7" s="18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1695,15 +1667,11 @@
         <v>116</v>
       </c>
       <c r="K8" s="8"/>
-      <c r="L8" t="s">
-        <v>153</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="18" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" ht="15.75">
+      <c r="L8" s="18" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="10" customFormat="1" ht="15.6">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1714,9 +1682,11 @@
         <v>137</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E9" s="11"/>
+        <v>337</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -1724,18 +1694,12 @@
       <c r="J9" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="L9" t="s">
-        <v>153</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="18" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75">
+      <c r="K9" s="11"/>
+      <c r="L9" s="18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1757,15 +1721,11 @@
         <v>118</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" t="s">
-        <v>153</v>
-      </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="18" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75">
+      <c r="L10" s="18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1776,9 +1736,11 @@
         <v>139</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>338</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>333</v>
+      </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1787,19 +1749,13 @@
         <v>119</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="L11" t="s">
-        <v>153</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75">
+        <v>242</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1819,12 +1775,8 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" t="s">
-        <v>153</v>
-      </c>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75">
+    </row>
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1844,12 +1796,8 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" t="s">
-        <v>153</v>
-      </c>
-      <c r="M13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75">
+    </row>
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1869,12 +1817,8 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" t="s">
-        <v>153</v>
-      </c>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75">
+    </row>
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1894,12 +1838,8 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" t="s">
-        <v>153</v>
-      </c>
-      <c r="M15" s="8"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75">
+    </row>
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1919,12 +1859,8 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" t="s">
-        <v>153</v>
-      </c>
-      <c r="M16" s="8"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75">
+    </row>
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1944,12 +1880,8 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" t="s">
-        <v>153</v>
-      </c>
-      <c r="M17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75">
+    </row>
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1969,12 +1901,8 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" t="s">
-        <v>153</v>
-      </c>
-      <c r="M18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75">
+    </row>
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1994,12 +1922,8 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" t="s">
-        <v>153</v>
-      </c>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75">
+    </row>
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -2019,12 +1943,8 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="L20" t="s">
-        <v>153</v>
-      </c>
-      <c r="M20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75">
+    </row>
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -2044,12 +1964,8 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" t="s">
-        <v>153</v>
-      </c>
-      <c r="M21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75">
+    </row>
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -2069,12 +1985,8 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" t="s">
-        <v>153</v>
-      </c>
-      <c r="M22" s="8"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75">
+    </row>
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -2094,12 +2006,8 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" t="s">
-        <v>153</v>
-      </c>
-      <c r="M23" s="8"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75">
+    </row>
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -2119,12 +2027,8 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
-      <c r="L24" t="s">
-        <v>153</v>
-      </c>
-      <c r="M24" s="8"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75">
+    </row>
+    <row r="25" spans="1:12" ht="15.6">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -2135,7 +2039,7 @@
         <v>37</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -2144,12 +2048,8 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" t="s">
-        <v>153</v>
-      </c>
-      <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75">
+    </row>
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -2170,18 +2070,14 @@
       <c r="J26" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" t="s">
-        <v>153</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="N26" s="18" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75">
+      <c r="K26" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -2203,15 +2099,11 @@
         <v>124</v>
       </c>
       <c r="K27" s="8"/>
-      <c r="L27" t="s">
-        <v>153</v>
-      </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="18" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.75">
+      <c r="L27" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -2232,18 +2124,14 @@
       <c r="J28" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="K28" s="8"/>
-      <c r="L28" t="s">
-        <v>153</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="N28" s="18" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15.75">
+      <c r="K28" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.6">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -2265,15 +2153,11 @@
         <v>97</v>
       </c>
       <c r="K29" s="8"/>
-      <c r="L29" t="s">
-        <v>153</v>
-      </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="18" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="15.75">
+      <c r="L29" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -2294,18 +2178,14 @@
       <c r="J30" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="K30" s="8"/>
-      <c r="L30" t="s">
-        <v>153</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="N30" s="18" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="15.75">
+      <c r="K30" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.6">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -2326,18 +2206,14 @@
       <c r="J31" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" t="s">
-        <v>153</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="N31" s="18" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15.75">
+      <c r="K31" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.6">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -2358,18 +2234,14 @@
       <c r="J32" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="K32" s="8"/>
-      <c r="L32" t="s">
-        <v>153</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="N32" s="18" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15.75">
+      <c r="K32" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -2391,15 +2263,11 @@
         <v>127</v>
       </c>
       <c r="K33" s="8"/>
-      <c r="L33" t="s">
-        <v>153</v>
-      </c>
-      <c r="M33" s="8"/>
-      <c r="N33" s="18" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="15.75">
+      <c r="L33" s="18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -2420,18 +2288,14 @@
       <c r="J34" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="K34" s="8"/>
-      <c r="L34" t="s">
-        <v>153</v>
-      </c>
-      <c r="M34" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="N34" s="18" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="15.75">
+      <c r="K34" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -2452,18 +2316,14 @@
       <c r="J35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="K35" s="8"/>
-      <c r="L35" t="s">
-        <v>153</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="N35" s="18" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="15.75">
+      <c r="K35" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -2484,18 +2344,14 @@
       <c r="J36" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="K36" s="8"/>
-      <c r="L36" t="s">
-        <v>153</v>
-      </c>
-      <c r="M36" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="N36" s="18" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="15.75">
+      <c r="K36" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -2516,18 +2372,14 @@
       <c r="J37" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="K37" s="8"/>
-      <c r="L37" t="s">
-        <v>153</v>
-      </c>
-      <c r="M37" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="N37" s="18" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="15.75">
+      <c r="K37" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="L37" s="18" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -2548,18 +2400,14 @@
       <c r="J38" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="K38" s="8"/>
-      <c r="L38" t="s">
-        <v>153</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="N38" s="18" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="15.75">
+      <c r="K38" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -2581,15 +2429,11 @@
         <v>146</v>
       </c>
       <c r="K39" s="8"/>
-      <c r="L39" t="s">
-        <v>153</v>
-      </c>
-      <c r="M39" s="8"/>
-      <c r="N39" s="18" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="15.75">
+      <c r="L39" s="18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.6">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -2611,15 +2455,11 @@
         <v>120</v>
       </c>
       <c r="K40" s="8"/>
-      <c r="L40" t="s">
-        <v>153</v>
-      </c>
-      <c r="M40" s="8"/>
-      <c r="N40" s="18" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="15.75">
+      <c r="L40" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2635,15 +2475,11 @@
       <c r="J41" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K41" s="8"/>
-      <c r="L41" t="s">
-        <v>153</v>
-      </c>
-      <c r="N41" s="18" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="15.75">
+      <c r="L41" s="18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -2654,25 +2490,22 @@
         <v>144</v>
       </c>
       <c r="D42" t="s">
-        <v>344</v>
+        <v>339</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>335</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="K42" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="L42" t="s">
-        <v>153</v>
-      </c>
-      <c r="M42" t="s">
-        <v>244</v>
-      </c>
-      <c r="N42" s="18" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="15.75">
+      <c r="K42" t="s">
+        <v>241</v>
+      </c>
+      <c r="L42" s="18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -2686,12 +2519,8 @@
         <v>67</v>
       </c>
       <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.75">
+    </row>
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -2705,12 +2534,8 @@
         <v>69</v>
       </c>
       <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="15.75">
+    </row>
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -2726,12 +2551,8 @@
       <c r="J45" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="K45" s="8"/>
-      <c r="L45" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="15.75">
+    </row>
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -2747,12 +2568,8 @@
       <c r="J46" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="K46" s="8"/>
-      <c r="L46" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="15.75">
+    </row>
+    <row r="47" spans="1:12" ht="15.6">
       <c r="A47" s="7">
         <v>1</v>
       </c>
@@ -2768,825 +2585,715 @@
       <c r="J47" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="K47" s="8"/>
-      <c r="L47" t="s">
-        <v>154</v>
-      </c>
-      <c r="M47" t="s">
-        <v>257</v>
-      </c>
-      <c r="N47" s="18" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="15.75">
+      <c r="K47" t="s">
+        <v>254</v>
+      </c>
+      <c r="L47" s="18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="7">
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>150</v>
       </c>
       <c r="D48" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J48" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="K48" s="8"/>
-      <c r="L48" t="s">
+      <c r="K48" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.6">
+      <c r="A49" s="7">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" t="s">
         <v>154</v>
       </c>
-      <c r="M48" t="s">
+      <c r="J49" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K49" t="s">
+        <v>257</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.6">
+      <c r="A50" s="7">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" t="s">
+        <v>157</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="K50" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" ht="15.75">
-      <c r="A49" s="7">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" t="s">
-        <v>157</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="K49" s="8"/>
-      <c r="L49" t="s">
-        <v>154</v>
-      </c>
-      <c r="M49" t="s">
+      <c r="L50" s="18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.6">
+      <c r="A51" s="7">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" t="s">
+        <v>158</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K51" t="s">
+        <v>259</v>
+      </c>
+      <c r="L51" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.6">
+      <c r="A52" s="7">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" t="s">
+        <v>162</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K52" t="s">
         <v>260</v>
       </c>
-      <c r="N49" s="18" t="s">
+      <c r="L52" s="18" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15.75">
-      <c r="A50" s="7">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>158</v>
-      </c>
-      <c r="C50" t="s">
-        <v>159</v>
-      </c>
-      <c r="D50" t="s">
-        <v>160</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="K50" s="8"/>
-      <c r="L50" t="s">
-        <v>154</v>
-      </c>
-      <c r="M50" t="s">
+    <row r="53" spans="1:12" ht="15.6">
+      <c r="A53" s="7">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>230</v>
+      </c>
+      <c r="D53" t="s">
+        <v>164</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K53" t="s">
         <v>261</v>
       </c>
-      <c r="N50" s="18" t="s">
+      <c r="L53" s="18" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15.75">
-      <c r="A51" s="7">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
-        <v>163</v>
-      </c>
-      <c r="C51" t="s">
-        <v>162</v>
-      </c>
-      <c r="D51" t="s">
-        <v>161</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="K51" s="8"/>
-      <c r="L51" t="s">
-        <v>154</v>
-      </c>
-      <c r="M51" t="s">
+    <row r="54" spans="1:12" ht="15.6">
+      <c r="A54" s="7">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" t="s">
+        <v>165</v>
+      </c>
+      <c r="J54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.6">
+      <c r="A55" s="7">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.6">
+      <c r="A56" s="7">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>227</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.6">
+      <c r="A57" s="7">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>233</v>
+      </c>
+      <c r="D57" t="s">
+        <v>170</v>
+      </c>
+      <c r="K57" t="s">
         <v>262</v>
       </c>
-      <c r="N51" s="18" t="s">
+      <c r="L57" s="18" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15.75">
-      <c r="A52" s="7">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>164</v>
-      </c>
-      <c r="C52" t="s">
-        <v>166</v>
-      </c>
-      <c r="D52" t="s">
-        <v>165</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="K52" s="8"/>
-      <c r="L52" t="s">
-        <v>154</v>
-      </c>
-      <c r="M52" t="s">
+    <row r="58" spans="1:12" ht="15.6">
+      <c r="A58" s="7">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" t="s">
+        <v>171</v>
+      </c>
+      <c r="J58" t="s">
+        <v>172</v>
+      </c>
+      <c r="K58" t="s">
         <v>263</v>
       </c>
-      <c r="N52" s="18" t="s">
+      <c r="L58" s="18" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15.75">
-      <c r="A53" s="7">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
-        <v>233</v>
-      </c>
-      <c r="D53" t="s">
-        <v>167</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="K53" s="8"/>
-      <c r="L53" t="s">
-        <v>154</v>
-      </c>
-      <c r="M53" t="s">
+    <row r="59" spans="1:12" ht="15.6">
+      <c r="A59" s="7">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" t="s">
+        <v>173</v>
+      </c>
+      <c r="J59" t="s">
+        <v>175</v>
+      </c>
+      <c r="K59" t="s">
         <v>264</v>
       </c>
-      <c r="N53" s="18" t="s">
+      <c r="L59" s="18" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15.75">
-      <c r="A54" s="7">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>169</v>
-      </c>
-      <c r="D54" t="s">
-        <v>168</v>
-      </c>
-      <c r="J54" t="s">
-        <v>169</v>
-      </c>
-      <c r="L54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="15.75">
-      <c r="A55" s="7">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="60" spans="1:12" ht="15.6">
+      <c r="A60" s="7">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" t="s">
+        <v>239</v>
+      </c>
+      <c r="F60" t="s">
+        <v>177</v>
+      </c>
+      <c r="J60" t="s">
+        <v>178</v>
+      </c>
+      <c r="K60" t="s">
+        <v>265</v>
+      </c>
+      <c r="L60" s="18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.6">
+      <c r="A61" s="7">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" t="s">
+        <v>181</v>
+      </c>
+      <c r="J61" t="s">
+        <v>179</v>
+      </c>
+      <c r="K61" t="s">
+        <v>251</v>
+      </c>
+      <c r="L61" s="18" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.6">
+      <c r="A62" s="7">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="L62" s="18" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.6">
+      <c r="A63" s="7">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" t="s">
+        <v>267</v>
+      </c>
+      <c r="I63" t="s">
+        <v>183</v>
+      </c>
+      <c r="J63" t="s">
+        <v>185</v>
+      </c>
+      <c r="K63" t="s">
+        <v>266</v>
+      </c>
+      <c r="L63" s="18" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.6">
+      <c r="A64" s="7">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>188</v>
+      </c>
+      <c r="D64" t="s">
+        <v>186</v>
+      </c>
+      <c r="K64" t="s">
+        <v>268</v>
+      </c>
+      <c r="L64" s="18" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.6">
+      <c r="A65" s="7">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" t="s">
+        <v>189</v>
+      </c>
+      <c r="J65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.6">
+      <c r="A66" s="7">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" t="s">
+        <v>193</v>
+      </c>
+      <c r="D66" t="s">
+        <v>191</v>
+      </c>
+      <c r="J66" t="s">
+        <v>192</v>
+      </c>
+      <c r="K66" t="s">
+        <v>269</v>
+      </c>
+      <c r="L66" s="18" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.6">
+      <c r="A67" s="7">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" t="s">
+        <v>196</v>
+      </c>
+      <c r="D67" t="s">
+        <v>194</v>
+      </c>
+      <c r="J67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.6">
+      <c r="A68" s="7">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
         <v>229</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="J55" t="s">
-        <v>171</v>
-      </c>
-      <c r="L55" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="15.75">
-      <c r="A56" s="7">
-        <v>1</v>
-      </c>
-      <c r="B56" t="s">
-        <v>230</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J56" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="K56" s="8"/>
-      <c r="L56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="15.75">
-      <c r="A57" s="7">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C68" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" t="s">
+        <v>197</v>
+      </c>
+      <c r="J68" t="s">
+        <v>152</v>
+      </c>
+      <c r="K68" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="15.6">
+      <c r="A69" s="7">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" t="s">
+        <v>199</v>
+      </c>
+      <c r="D69" t="s">
+        <v>201</v>
+      </c>
+      <c r="K69" t="s">
+        <v>271</v>
+      </c>
+      <c r="L69" s="18" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="15.6">
+      <c r="A70" s="7">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>202</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15.6">
+      <c r="A71" s="7">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>220</v>
+      </c>
+      <c r="C71" t="s">
+        <v>204</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E71" s="13"/>
+      <c r="K71" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L71" s="18" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15.6">
+      <c r="A72" s="7">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>237</v>
+      </c>
+      <c r="C72" t="s">
+        <v>235</v>
+      </c>
+      <c r="D72" s="10" t="s">
         <v>236</v>
-      </c>
-      <c r="D57" t="s">
-        <v>173</v>
-      </c>
-      <c r="L57" t="s">
-        <v>154</v>
-      </c>
-      <c r="M57" t="s">
-        <v>265</v>
-      </c>
-      <c r="N57" s="18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="15.75">
-      <c r="A58" s="7">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
-        <v>175</v>
-      </c>
-      <c r="D58" t="s">
-        <v>174</v>
-      </c>
-      <c r="J58" t="s">
-        <v>175</v>
-      </c>
-      <c r="L58" t="s">
-        <v>154</v>
-      </c>
-      <c r="M58" t="s">
-        <v>266</v>
-      </c>
-      <c r="N58" s="18" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="15.75">
-      <c r="A59" s="7">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>178</v>
-      </c>
-      <c r="C59" t="s">
-        <v>177</v>
-      </c>
-      <c r="D59" t="s">
-        <v>176</v>
-      </c>
-      <c r="J59" t="s">
-        <v>178</v>
-      </c>
-      <c r="L59" t="s">
-        <v>154</v>
-      </c>
-      <c r="M59" t="s">
-        <v>267</v>
-      </c>
-      <c r="N59" s="18" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="15.75">
-      <c r="A60" s="7">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
-        <v>181</v>
-      </c>
-      <c r="D60" t="s">
-        <v>242</v>
-      </c>
-      <c r="F60" t="s">
-        <v>180</v>
-      </c>
-      <c r="J60" t="s">
-        <v>181</v>
-      </c>
-      <c r="L60" t="s">
-        <v>154</v>
-      </c>
-      <c r="M60" t="s">
-        <v>268</v>
-      </c>
-      <c r="N60" s="18" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="15.75">
-      <c r="A61" s="7">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
-        <v>231</v>
-      </c>
-      <c r="C61" t="s">
-        <v>183</v>
-      </c>
-      <c r="D61" t="s">
-        <v>184</v>
-      </c>
-      <c r="J61" t="s">
-        <v>182</v>
-      </c>
-      <c r="L61" t="s">
-        <v>154</v>
-      </c>
-      <c r="M61" t="s">
-        <v>254</v>
-      </c>
-      <c r="N61" s="18" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="15.75">
-      <c r="A62" s="7">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s">
-        <v>185</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="L62" t="s">
-        <v>154</v>
-      </c>
-      <c r="N62" s="18" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="15.75">
-      <c r="A63" s="7">
-        <v>1</v>
-      </c>
-      <c r="B63" t="s">
-        <v>188</v>
-      </c>
-      <c r="D63" t="s">
-        <v>270</v>
-      </c>
-      <c r="I63" t="s">
-        <v>186</v>
-      </c>
-      <c r="J63" t="s">
-        <v>188</v>
-      </c>
-      <c r="L63" t="s">
-        <v>154</v>
-      </c>
-      <c r="M63" t="s">
-        <v>269</v>
-      </c>
-      <c r="N63" s="18" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="15.75">
-      <c r="A64" s="7">
-        <v>1</v>
-      </c>
-      <c r="B64" t="s">
-        <v>190</v>
-      </c>
-      <c r="C64" t="s">
-        <v>191</v>
-      </c>
-      <c r="D64" t="s">
-        <v>189</v>
-      </c>
-      <c r="L64" t="s">
-        <v>154</v>
-      </c>
-      <c r="M64" t="s">
-        <v>271</v>
-      </c>
-      <c r="N64" s="18" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="15.75">
-      <c r="A65" s="7">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
-        <v>193</v>
-      </c>
-      <c r="D65" t="s">
-        <v>192</v>
-      </c>
-      <c r="J65" t="s">
-        <v>193</v>
-      </c>
-      <c r="L65" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="15.75">
-      <c r="A66" s="7">
-        <v>1</v>
-      </c>
-      <c r="B66" t="s">
-        <v>195</v>
-      </c>
-      <c r="C66" t="s">
-        <v>196</v>
-      </c>
-      <c r="D66" t="s">
-        <v>194</v>
-      </c>
-      <c r="J66" t="s">
-        <v>195</v>
-      </c>
-      <c r="L66" t="s">
-        <v>154</v>
-      </c>
-      <c r="M66" t="s">
-        <v>272</v>
-      </c>
-      <c r="N66" s="18" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="15.75">
-      <c r="A67" s="7">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s">
-        <v>198</v>
-      </c>
-      <c r="C67" t="s">
-        <v>199</v>
-      </c>
-      <c r="D67" t="s">
-        <v>197</v>
-      </c>
-      <c r="J67" t="s">
-        <v>198</v>
-      </c>
-      <c r="L67" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="15.75">
-      <c r="A68" s="7">
-        <v>1</v>
-      </c>
-      <c r="B68" t="s">
-        <v>232</v>
-      </c>
-      <c r="C68" t="s">
-        <v>201</v>
-      </c>
-      <c r="D68" t="s">
-        <v>200</v>
-      </c>
-      <c r="J68" t="s">
-        <v>155</v>
-      </c>
-      <c r="L68" t="s">
-        <v>154</v>
-      </c>
-      <c r="M68" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="15.75">
-      <c r="A69" s="7">
-        <v>1</v>
-      </c>
-      <c r="B69" t="s">
-        <v>203</v>
-      </c>
-      <c r="C69" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" t="s">
-        <v>204</v>
-      </c>
-      <c r="L69" t="s">
-        <v>154</v>
-      </c>
-      <c r="M69" t="s">
-        <v>274</v>
-      </c>
-      <c r="N69" s="18" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="15.75">
-      <c r="A70" s="7">
-        <v>1</v>
-      </c>
-      <c r="B70" t="s">
-        <v>205</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="L70" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="15.75">
-      <c r="A71" s="7">
-        <v>1</v>
-      </c>
-      <c r="B71" t="s">
-        <v>223</v>
-      </c>
-      <c r="C71" t="s">
-        <v>207</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="E71" s="13"/>
-      <c r="L71" t="s">
-        <v>154</v>
-      </c>
-      <c r="M71" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="N71" s="18" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" ht="15.75">
-      <c r="A72" s="7">
-        <v>1</v>
-      </c>
-      <c r="B72" t="s">
-        <v>240</v>
-      </c>
-      <c r="C72" t="s">
-        <v>238</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>239</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="15"/>
       <c r="H72" s="15"/>
-      <c r="L72" t="s">
-        <v>154</v>
-      </c>
-      <c r="M72" t="s">
+      <c r="K72" t="s">
+        <v>274</v>
+      </c>
+      <c r="L72" s="18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="15.6">
+      <c r="A73" s="7">
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>231</v>
+      </c>
+      <c r="C73" t="s">
+        <v>205</v>
+      </c>
+      <c r="D73" t="s">
+        <v>275</v>
+      </c>
+      <c r="K73" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="15.6">
+      <c r="A74" s="7">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>206</v>
+      </c>
+      <c r="C74" t="s">
+        <v>208</v>
+      </c>
+      <c r="D74" t="s">
+        <v>207</v>
+      </c>
+      <c r="J74" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="K74" t="s">
+        <v>276</v>
+      </c>
+      <c r="L74" s="18" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15.6">
+      <c r="A75" s="7">
+        <v>1</v>
+      </c>
+      <c r="B75" t="s">
+        <v>210</v>
+      </c>
+      <c r="D75" t="s">
+        <v>211</v>
+      </c>
+      <c r="E75" t="s">
+        <v>209</v>
+      </c>
+      <c r="J75" t="s">
+        <v>210</v>
+      </c>
+      <c r="K75" t="s">
         <v>277</v>
       </c>
-      <c r="N72" s="18" t="s">
+    </row>
+    <row r="76" spans="1:12" ht="15.6">
+      <c r="A76" s="7">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>213</v>
+      </c>
+      <c r="D76" t="s">
+        <v>212</v>
+      </c>
+      <c r="H76" t="s">
+        <v>215</v>
+      </c>
+      <c r="J76" t="s">
+        <v>213</v>
+      </c>
+      <c r="K76" t="s">
+        <v>278</v>
+      </c>
+      <c r="L76" s="18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15.6">
+      <c r="A77" s="7">
+        <v>1</v>
+      </c>
+      <c r="B77" t="s">
+        <v>232</v>
+      </c>
+      <c r="D77" t="s">
+        <v>216</v>
+      </c>
+      <c r="G77" s="14"/>
+      <c r="K77" s="19" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15.6">
+      <c r="A78" s="7">
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>217</v>
+      </c>
+      <c r="D78" t="s">
+        <v>281</v>
+      </c>
+      <c r="G78" t="s">
+        <v>219</v>
+      </c>
+      <c r="J78" t="s">
+        <v>217</v>
+      </c>
+      <c r="K78" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="15.6">
+      <c r="A79" s="7">
+        <v>1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>222</v>
+      </c>
+      <c r="D79" t="s">
+        <v>221</v>
+      </c>
+      <c r="I79" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="J79" t="s">
+        <v>222</v>
+      </c>
+      <c r="K79" t="s">
+        <v>282</v>
+      </c>
+      <c r="L79" s="18" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15.75">
-      <c r="A73" s="7">
-        <v>1</v>
-      </c>
-      <c r="B73" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" t="s">
-        <v>208</v>
-      </c>
-      <c r="D73" t="s">
-        <v>278</v>
-      </c>
-      <c r="L73" t="s">
-        <v>154</v>
-      </c>
-      <c r="M73" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="15.75">
-      <c r="A74" s="7">
-        <v>1</v>
-      </c>
-      <c r="B74" t="s">
-        <v>209</v>
-      </c>
-      <c r="C74" t="s">
-        <v>211</v>
-      </c>
-      <c r="D74" t="s">
-        <v>210</v>
-      </c>
-      <c r="J74" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="K74" s="13"/>
-      <c r="L74" t="s">
-        <v>154</v>
-      </c>
-      <c r="M74" t="s">
-        <v>279</v>
-      </c>
-      <c r="N74" s="18" t="s">
+    <row r="80" spans="1:12" ht="15.6">
+      <c r="A80" s="7">
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>224</v>
+      </c>
+      <c r="D80" t="s">
+        <v>284</v>
+      </c>
+      <c r="I80" t="s">
+        <v>223</v>
+      </c>
+      <c r="J80" t="s">
+        <v>224</v>
+      </c>
+      <c r="K80" t="s">
+        <v>283</v>
+      </c>
+      <c r="L80" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15.75">
-      <c r="A75" s="7">
-        <v>1</v>
-      </c>
-      <c r="B75" t="s">
-        <v>213</v>
-      </c>
-      <c r="D75" t="s">
-        <v>214</v>
-      </c>
-      <c r="E75" t="s">
-        <v>212</v>
-      </c>
-      <c r="J75" t="s">
-        <v>213</v>
-      </c>
-      <c r="L75" t="s">
-        <v>154</v>
-      </c>
-      <c r="M75" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" ht="15.75">
-      <c r="A76" s="7">
-        <v>1</v>
-      </c>
-      <c r="B76" t="s">
-        <v>216</v>
-      </c>
-      <c r="D76" t="s">
-        <v>215</v>
-      </c>
-      <c r="H76" t="s">
-        <v>218</v>
-      </c>
-      <c r="J76" t="s">
-        <v>216</v>
-      </c>
-      <c r="L76" t="s">
-        <v>154</v>
-      </c>
-      <c r="M76" t="s">
-        <v>281</v>
-      </c>
-      <c r="N76" s="18" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="15.75">
-      <c r="A77" s="7">
-        <v>1</v>
-      </c>
-      <c r="B77" t="s">
-        <v>235</v>
-      </c>
-      <c r="D77" t="s">
-        <v>219</v>
-      </c>
-      <c r="G77" s="14"/>
-      <c r="L77" t="s">
-        <v>154</v>
-      </c>
-      <c r="M77" s="19" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="15.75">
-      <c r="A78" s="7">
-        <v>1</v>
-      </c>
-      <c r="B78" t="s">
-        <v>220</v>
-      </c>
-      <c r="D78" t="s">
-        <v>284</v>
-      </c>
-      <c r="G78" t="s">
-        <v>222</v>
-      </c>
-      <c r="J78" t="s">
-        <v>220</v>
-      </c>
-      <c r="L78" t="s">
-        <v>154</v>
-      </c>
-      <c r="M78" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="15.75">
-      <c r="A79" s="7">
-        <v>1</v>
-      </c>
-      <c r="B79" t="s">
-        <v>225</v>
-      </c>
-      <c r="D79" t="s">
-        <v>224</v>
-      </c>
-      <c r="I79" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="J79" t="s">
-        <v>225</v>
-      </c>
-      <c r="L79" t="s">
-        <v>154</v>
-      </c>
-      <c r="M79" t="s">
-        <v>285</v>
-      </c>
-      <c r="N79" s="18" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="15.75">
-      <c r="A80" s="7">
-        <v>1</v>
-      </c>
-      <c r="B80" t="s">
-        <v>227</v>
-      </c>
-      <c r="D80" t="s">
-        <v>287</v>
-      </c>
-      <c r="I80" t="s">
-        <v>226</v>
-      </c>
-      <c r="J80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L80" t="s">
-        <v>154</v>
-      </c>
-      <c r="M80" t="s">
-        <v>286</v>
-      </c>
-      <c r="N80" s="18" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="15.75">
+    <row r="81" spans="1:1" ht="15.6">
       <c r="A81" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="A5:L80"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1"/>
-    <hyperlink ref="N7" r:id="rId2"/>
-    <hyperlink ref="N8" r:id="rId3"/>
-    <hyperlink ref="N9" r:id="rId4"/>
-    <hyperlink ref="N10" r:id="rId5"/>
-    <hyperlink ref="N11" r:id="rId6"/>
-    <hyperlink ref="N26" r:id="rId7"/>
-    <hyperlink ref="N27" r:id="rId8"/>
-    <hyperlink ref="N28" r:id="rId9"/>
-    <hyperlink ref="N35" r:id="rId10"/>
-    <hyperlink ref="N33" r:id="rId11"/>
-    <hyperlink ref="N36" r:id="rId12"/>
-    <hyperlink ref="N37" r:id="rId13"/>
-    <hyperlink ref="N29" r:id="rId14"/>
-    <hyperlink ref="N30" r:id="rId15"/>
-    <hyperlink ref="N31" r:id="rId16"/>
-    <hyperlink ref="N32" r:id="rId17"/>
-    <hyperlink ref="N34" r:id="rId18"/>
-    <hyperlink ref="N38" r:id="rId19"/>
-    <hyperlink ref="N39" r:id="rId20"/>
-    <hyperlink ref="N40" r:id="rId21"/>
-    <hyperlink ref="N41" r:id="rId22"/>
-    <hyperlink ref="N42" r:id="rId23"/>
-    <hyperlink ref="N47" r:id="rId24"/>
-    <hyperlink ref="N49" r:id="rId25"/>
-    <hyperlink ref="N50" r:id="rId26"/>
-    <hyperlink ref="N51" r:id="rId27"/>
-    <hyperlink ref="N52" r:id="rId28"/>
-    <hyperlink ref="N53" r:id="rId29"/>
-    <hyperlink ref="N57" r:id="rId30"/>
-    <hyperlink ref="N58" r:id="rId31"/>
-    <hyperlink ref="N59" r:id="rId32"/>
-    <hyperlink ref="N60" r:id="rId33"/>
-    <hyperlink ref="N61" r:id="rId34"/>
-    <hyperlink ref="N62" r:id="rId35"/>
-    <hyperlink ref="N63" r:id="rId36"/>
-    <hyperlink ref="N64" r:id="rId37"/>
-    <hyperlink ref="N66" r:id="rId38"/>
-    <hyperlink ref="N69" r:id="rId39"/>
-    <hyperlink ref="N71" r:id="rId40"/>
-    <hyperlink ref="N72" r:id="rId41"/>
-    <hyperlink ref="N74" r:id="rId42"/>
-    <hyperlink ref="N76" r:id="rId43"/>
-    <hyperlink ref="M77" r:id="rId44"/>
-    <hyperlink ref="N79" r:id="rId45"/>
-    <hyperlink ref="N80" r:id="rId46"/>
+    <hyperlink ref="L6" r:id="rId1"/>
+    <hyperlink ref="L7" r:id="rId2"/>
+    <hyperlink ref="L8" r:id="rId3"/>
+    <hyperlink ref="L9" r:id="rId4"/>
+    <hyperlink ref="L10" r:id="rId5"/>
+    <hyperlink ref="L11" r:id="rId6"/>
+    <hyperlink ref="L26" r:id="rId7"/>
+    <hyperlink ref="L27" r:id="rId8"/>
+    <hyperlink ref="L28" r:id="rId9"/>
+    <hyperlink ref="L35" r:id="rId10"/>
+    <hyperlink ref="L33" r:id="rId11"/>
+    <hyperlink ref="L36" r:id="rId12"/>
+    <hyperlink ref="L37" r:id="rId13"/>
+    <hyperlink ref="L29" r:id="rId14"/>
+    <hyperlink ref="L30" r:id="rId15"/>
+    <hyperlink ref="L31" r:id="rId16"/>
+    <hyperlink ref="L32" r:id="rId17"/>
+    <hyperlink ref="L34" r:id="rId18"/>
+    <hyperlink ref="L38" r:id="rId19"/>
+    <hyperlink ref="L39" r:id="rId20"/>
+    <hyperlink ref="L40" r:id="rId21"/>
+    <hyperlink ref="L41" r:id="rId22"/>
+    <hyperlink ref="L42" r:id="rId23"/>
+    <hyperlink ref="L47" r:id="rId24"/>
+    <hyperlink ref="L49" r:id="rId25"/>
+    <hyperlink ref="L50" r:id="rId26"/>
+    <hyperlink ref="L51" r:id="rId27"/>
+    <hyperlink ref="L52" r:id="rId28"/>
+    <hyperlink ref="L53" r:id="rId29"/>
+    <hyperlink ref="L57" r:id="rId30"/>
+    <hyperlink ref="L58" r:id="rId31"/>
+    <hyperlink ref="L59" r:id="rId32"/>
+    <hyperlink ref="L60" r:id="rId33"/>
+    <hyperlink ref="L61" r:id="rId34"/>
+    <hyperlink ref="L62" r:id="rId35"/>
+    <hyperlink ref="L63" r:id="rId36"/>
+    <hyperlink ref="L64" r:id="rId37"/>
+    <hyperlink ref="L66" r:id="rId38"/>
+    <hyperlink ref="L69" r:id="rId39"/>
+    <hyperlink ref="L71" r:id="rId40"/>
+    <hyperlink ref="L72" r:id="rId41"/>
+    <hyperlink ref="L74" r:id="rId42"/>
+    <hyperlink ref="L76" r:id="rId43"/>
+    <hyperlink ref="K77" r:id="rId44"/>
+    <hyperlink ref="L79" r:id="rId45"/>
+    <hyperlink ref="L80" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId47"/>

</xml_diff>

<commit_message>
Updated funders and institutions
</commit_message>
<xml_diff>
--- a/data/excel/funders.xlsx
+++ b/data/excel/funders.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\taxonomie\současné_hotové\aktualne_pouzite_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\metadatové modely\nr-github\nr-taxonomies\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4746160-155B-4630-8D64-BDDABCD34933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12630" tabRatio="500"/>
+    <workbookView xWindow="33255" yWindow="690" windowWidth="21600" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nr" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="356">
   <si>
     <t>code</t>
   </si>
@@ -1071,12 +1072,36 @@
   </si>
   <si>
     <t>formerTitles_en_0</t>
+  </si>
+  <si>
+    <t>UPCE</t>
+  </si>
+  <si>
+    <t>Univerzita Pardubice</t>
+  </si>
+  <si>
+    <t>University of Pardubice</t>
+  </si>
+  <si>
+    <t>https://ror.org/01chzd453</t>
+  </si>
+  <si>
+    <t>APVV</t>
+  </si>
+  <si>
+    <t>Slovak Research and Development Agency</t>
+  </si>
+  <si>
+    <t>Agentúra na podporu výskumu a vývoja</t>
+  </si>
+  <si>
+    <t>https://ror.org/037nx0e70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1156,7 +1181,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1167,19 +1192,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1187,20 +1205,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hypertextový odkaz" xfId="2" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Normální 2" xfId="1"/>
+    <cellStyle name="Normální 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1488,13 +1502,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15"/>
@@ -1596,16 +1610,16 @@
       <c r="J5" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>152</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="4" t="s">
         <v>346</v>
       </c>
     </row>
@@ -1613,33 +1627,33 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="4" t="s">
         <v>337</v>
       </c>
       <c r="L6" t="s">
         <v>153</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="12" t="s">
         <v>289</v>
       </c>
     </row>
@@ -1647,29 +1661,29 @@
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="8"/>
+      <c r="K7" s="6"/>
       <c r="L7" t="s">
         <v>153</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="18" t="s">
+      <c r="M7" s="6"/>
+      <c r="N7" s="12" t="s">
         <v>290</v>
       </c>
     </row>
@@ -1677,61 +1691,61 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="K8" s="8"/>
+      <c r="K8" s="6"/>
       <c r="L8" t="s">
         <v>153</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="18" t="s">
+      <c r="M8" s="6"/>
+      <c r="N8" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" ht="15.75">
+    <row r="9" spans="1:14" ht="15.75">
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="8" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="6" t="s">
         <v>339</v>
       </c>
       <c r="L9" t="s">
         <v>153</v>
       </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="18" t="s">
+      <c r="M9" s="6"/>
+      <c r="N9" s="12" t="s">
         <v>292</v>
       </c>
     </row>
@@ -1739,29 +1753,29 @@
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="K10" s="8"/>
+      <c r="K10" s="6"/>
       <c r="L10" t="s">
         <v>153</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="18" t="s">
+      <c r="M10" s="6"/>
+      <c r="N10" s="12" t="s">
         <v>293</v>
       </c>
     </row>
@@ -1769,33 +1783,33 @@
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="6" t="s">
         <v>338</v>
       </c>
       <c r="L11" t="s">
         <v>153</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="12" t="s">
         <v>294</v>
       </c>
     </row>
@@ -1803,381 +1817,381 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" t="s">
         <v>153</v>
       </c>
-      <c r="M12" s="8"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:14" ht="15.75">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
       <c r="L13" t="s">
         <v>153</v>
       </c>
-      <c r="M13" s="8"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:14" ht="15.75">
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" t="s">
         <v>153</v>
       </c>
-      <c r="M14" s="8"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:14" ht="15.75">
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
       <c r="L15" t="s">
         <v>153</v>
       </c>
-      <c r="M15" s="8"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:14" ht="15.75">
       <c r="A16" s="1">
         <v>1</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="L16" t="s">
         <v>153</v>
       </c>
-      <c r="M16" s="8"/>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:14" ht="15.75">
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
       <c r="L17" t="s">
         <v>153</v>
       </c>
-      <c r="M17" s="8"/>
+      <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:14" ht="15.75">
       <c r="A18" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" t="s">
         <v>153</v>
       </c>
-      <c r="M18" s="8"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:14" ht="15.75">
       <c r="A19" s="1">
         <v>1</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" t="s">
         <v>153</v>
       </c>
-      <c r="M19" s="8"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:14" ht="15.75">
       <c r="A20" s="1">
         <v>1</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
       <c r="L20" t="s">
         <v>153</v>
       </c>
-      <c r="M20" s="8"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:14" ht="15.75">
       <c r="A21" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" t="s">
         <v>153</v>
       </c>
-      <c r="M21" s="8"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:14" ht="15.75">
       <c r="A22" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
       <c r="L22" t="s">
         <v>153</v>
       </c>
-      <c r="M22" s="8"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:14" ht="15.75">
       <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
       <c r="L23" t="s">
         <v>153</v>
       </c>
-      <c r="M23" s="8"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:14" ht="15.75">
       <c r="A24" s="1">
         <v>1</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
       <c r="L24" t="s">
         <v>153</v>
       </c>
-      <c r="M24" s="8"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" spans="1:14" ht="15.75">
       <c r="A25" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
       <c r="L25" t="s">
         <v>153</v>
       </c>
-      <c r="M25" s="8"/>
+      <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:14" ht="15.75">
       <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8" t="s">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="K26" s="8"/>
+      <c r="K26" s="6"/>
       <c r="L26" t="s">
         <v>153</v>
       </c>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="N26" s="18" t="s">
+      <c r="N26" s="12" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2185,29 +2199,29 @@
       <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="K27" s="8"/>
+      <c r="K27" s="6"/>
       <c r="L27" t="s">
         <v>153</v>
       </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="18" t="s">
+      <c r="M27" s="6"/>
+      <c r="N27" s="12" t="s">
         <v>296</v>
       </c>
     </row>
@@ -2215,31 +2229,31 @@
       <c r="A28" s="1">
         <v>1</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="K28" s="8"/>
+      <c r="K28" s="6"/>
       <c r="L28" t="s">
         <v>153</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="M28" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="N28" s="18" t="s">
+      <c r="N28" s="12" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2247,29 +2261,29 @@
       <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="K29" s="8"/>
+      <c r="K29" s="6"/>
       <c r="L29" t="s">
         <v>153</v>
       </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="18" t="s">
+      <c r="M29" s="6"/>
+      <c r="N29" s="12" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2277,31 +2291,31 @@
       <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8" t="s">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="K30" s="8"/>
+      <c r="K30" s="6"/>
       <c r="L30" t="s">
         <v>153</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="N30" s="18" t="s">
+      <c r="N30" s="12" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2309,31 +2323,31 @@
       <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8" t="s">
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="K31" s="8"/>
+      <c r="K31" s="6"/>
       <c r="L31" t="s">
         <v>153</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="M31" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="N31" s="18" t="s">
+      <c r="N31" s="12" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2341,31 +2355,31 @@
       <c r="A32" s="1">
         <v>1</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8" t="s">
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="K32" s="8"/>
+      <c r="K32" s="6"/>
       <c r="L32" t="s">
         <v>153</v>
       </c>
-      <c r="M32" s="8" t="s">
+      <c r="M32" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="N32" s="18" t="s">
+      <c r="N32" s="12" t="s">
         <v>305</v>
       </c>
     </row>
@@ -2373,29 +2387,29 @@
       <c r="A33" s="1">
         <v>1</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8" t="s">
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="K33" s="8"/>
+      <c r="K33" s="6"/>
       <c r="L33" t="s">
         <v>153</v>
       </c>
-      <c r="M33" s="8"/>
-      <c r="N33" s="18" t="s">
+      <c r="M33" s="6"/>
+      <c r="N33" s="12" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2403,31 +2417,31 @@
       <c r="A34" s="1">
         <v>1</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="K34" s="8"/>
+      <c r="K34" s="6"/>
       <c r="L34" t="s">
         <v>153</v>
       </c>
-      <c r="M34" s="8" t="s">
+      <c r="M34" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="N34" s="18" t="s">
+      <c r="N34" s="12" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2435,31 +2449,31 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8" t="s">
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="K35" s="8"/>
+      <c r="K35" s="6"/>
       <c r="L35" t="s">
         <v>153</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M35" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="N35" s="18" t="s">
+      <c r="N35" s="12" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2467,31 +2481,31 @@
       <c r="A36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8" t="s">
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="K36" s="8"/>
+      <c r="K36" s="6"/>
       <c r="L36" t="s">
         <v>153</v>
       </c>
-      <c r="M36" s="8" t="s">
+      <c r="M36" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="N36" s="18" t="s">
+      <c r="N36" s="12" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2499,31 +2513,31 @@
       <c r="A37" s="1">
         <v>1</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="K37" s="8"/>
+      <c r="K37" s="6"/>
       <c r="L37" t="s">
         <v>153</v>
       </c>
-      <c r="M37" s="8" t="s">
+      <c r="M37" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="N37" s="18" t="s">
+      <c r="N37" s="12" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2531,31 +2545,31 @@
       <c r="A38" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8" t="s">
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="K38" s="8"/>
+      <c r="K38" s="6"/>
       <c r="L38" t="s">
         <v>153</v>
       </c>
-      <c r="M38" s="8" t="s">
+      <c r="M38" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="N38" s="18" t="s">
+      <c r="N38" s="12" t="s">
         <v>307</v>
       </c>
     </row>
@@ -2563,29 +2577,29 @@
       <c r="A39" s="1">
         <v>1</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8" t="s">
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K39" s="8"/>
+      <c r="K39" s="6"/>
       <c r="L39" t="s">
         <v>153</v>
       </c>
-      <c r="M39" s="8"/>
-      <c r="N39" s="18" t="s">
+      <c r="M39" s="6"/>
+      <c r="N39" s="12" t="s">
         <v>308</v>
       </c>
     </row>
@@ -2593,29 +2607,29 @@
       <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8" t="s">
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="K40" s="8"/>
+      <c r="K40" s="6"/>
       <c r="L40" t="s">
         <v>153</v>
       </c>
-      <c r="M40" s="8"/>
-      <c r="N40" s="18" t="s">
+      <c r="M40" s="6"/>
+      <c r="N40" s="12" t="s">
         <v>309</v>
       </c>
     </row>
@@ -2626,20 +2640,20 @@
       <c r="B41" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" t="s">
         <v>143</v>
       </c>
       <c r="D41" t="s">
         <v>65</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J41" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="K41" s="8"/>
+      <c r="K41" s="6"/>
       <c r="L41" t="s">
         <v>153</v>
       </c>
-      <c r="N41" s="18" t="s">
+      <c r="N41" s="12" t="s">
         <v>310</v>
       </c>
     </row>
@@ -2650,16 +2664,16 @@
       <c r="B42" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" t="s">
         <v>144</v>
       </c>
       <c r="D42" t="s">
         <v>344</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="J42" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="K42" s="6" t="s">
         <v>340</v>
       </c>
       <c r="L42" t="s">
@@ -2668,7 +2682,7 @@
       <c r="M42" t="s">
         <v>244</v>
       </c>
-      <c r="N42" s="18" t="s">
+      <c r="N42" s="12" t="s">
         <v>311</v>
       </c>
     </row>
@@ -2679,14 +2693,14 @@
       <c r="B43" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" t="s">
         <v>66</v>
       </c>
       <c r="D43" t="s">
         <v>67</v>
       </c>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
       <c r="L43" t="s">
         <v>153</v>
       </c>
@@ -2698,14 +2712,14 @@
       <c r="B44" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" t="s">
         <v>68</v>
       </c>
       <c r="D44" t="s">
         <v>69</v>
       </c>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
       <c r="L44" t="s">
         <v>153</v>
       </c>
@@ -2717,16 +2731,16 @@
       <c r="B45" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
         <v>71</v>
       </c>
-      <c r="J45" s="8" t="s">
+      <c r="J45" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="K45" s="8"/>
+      <c r="K45" s="6"/>
       <c r="L45" t="s">
         <v>153</v>
       </c>
@@ -2738,64 +2752,64 @@
       <c r="B46" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" t="s">
         <v>72</v>
       </c>
       <c r="D46" t="s">
         <v>73</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J46" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="K46" s="8"/>
+      <c r="K46" s="6"/>
       <c r="L46" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75">
-      <c r="A47" s="7">
+      <c r="A47" s="4">
         <v>1</v>
       </c>
       <c r="B47" t="s">
         <v>148</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" t="s">
         <v>147</v>
       </c>
       <c r="D47" t="s">
         <v>149</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="J47" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="K47" s="8"/>
+      <c r="K47" s="6"/>
       <c r="L47" t="s">
         <v>154</v>
       </c>
       <c r="M47" t="s">
         <v>257</v>
       </c>
-      <c r="N47" s="18" t="s">
+      <c r="N47" s="12" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75">
-      <c r="A48" s="7">
+      <c r="A48" s="4">
         <v>1</v>
       </c>
       <c r="B48" t="s">
         <v>228</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" t="s">
         <v>150</v>
       </c>
       <c r="D48" t="s">
         <v>259</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="J48" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="K48" s="8"/>
+      <c r="K48" s="6"/>
       <c r="L48" t="s">
         <v>154</v>
       </c>
@@ -2804,7 +2818,7 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="15.75">
-      <c r="A49" s="7">
+      <c r="A49" s="4">
         <v>1</v>
       </c>
       <c r="B49" t="s">
@@ -2813,22 +2827,22 @@
       <c r="D49" t="s">
         <v>157</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="K49" s="8"/>
+      <c r="K49" s="6"/>
       <c r="L49" t="s">
         <v>154</v>
       </c>
       <c r="M49" t="s">
         <v>260</v>
       </c>
-      <c r="N49" s="18" t="s">
+      <c r="N49" s="12" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75">
-      <c r="A50" s="7">
+      <c r="A50" s="4">
         <v>1</v>
       </c>
       <c r="B50" t="s">
@@ -2840,22 +2854,22 @@
       <c r="D50" t="s">
         <v>160</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="J50" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="K50" s="8"/>
+      <c r="K50" s="6"/>
       <c r="L50" t="s">
         <v>154</v>
       </c>
       <c r="M50" t="s">
         <v>261</v>
       </c>
-      <c r="N50" s="18" t="s">
+      <c r="N50" s="12" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="15.75">
-      <c r="A51" s="7">
+      <c r="A51" s="4">
         <v>1</v>
       </c>
       <c r="B51" t="s">
@@ -2867,22 +2881,22 @@
       <c r="D51" t="s">
         <v>161</v>
       </c>
-      <c r="J51" s="8" t="s">
+      <c r="J51" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K51" s="8"/>
+      <c r="K51" s="6"/>
       <c r="L51" t="s">
         <v>154</v>
       </c>
       <c r="M51" t="s">
         <v>262</v>
       </c>
-      <c r="N51" s="18" t="s">
+      <c r="N51" s="12" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15.75">
-      <c r="A52" s="7">
+      <c r="A52" s="4">
         <v>1</v>
       </c>
       <c r="B52" t="s">
@@ -2894,22 +2908,22 @@
       <c r="D52" t="s">
         <v>165</v>
       </c>
-      <c r="J52" s="8" t="s">
+      <c r="J52" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="K52" s="8"/>
+      <c r="K52" s="6"/>
       <c r="L52" t="s">
         <v>154</v>
       </c>
       <c r="M52" t="s">
         <v>263</v>
       </c>
-      <c r="N52" s="18" t="s">
+      <c r="N52" s="12" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="15.75">
-      <c r="A53" s="7">
+      <c r="A53" s="4">
         <v>1</v>
       </c>
       <c r="B53" t="s">
@@ -2918,22 +2932,22 @@
       <c r="D53" t="s">
         <v>167</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="J53" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="K53" s="8"/>
+      <c r="K53" s="6"/>
       <c r="L53" t="s">
         <v>154</v>
       </c>
       <c r="M53" t="s">
         <v>264</v>
       </c>
-      <c r="N53" s="18" t="s">
+      <c r="N53" s="12" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15.75">
-      <c r="A54" s="7">
+      <c r="A54" s="4">
         <v>1</v>
       </c>
       <c r="B54" t="s">
@@ -2950,13 +2964,13 @@
       </c>
     </row>
     <row r="55" spans="1:14" ht="15.75">
-      <c r="A55" s="7">
+      <c r="A55" s="4">
         <v>1</v>
       </c>
       <c r="B55" t="s">
         <v>229</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" t="s">
         <v>170</v>
       </c>
       <c r="J55" t="s">
@@ -2967,25 +2981,25 @@
       </c>
     </row>
     <row r="56" spans="1:14" ht="15.75">
-      <c r="A56" s="7">
+      <c r="A56" s="4">
         <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>230</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="J56" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="K56" s="8"/>
+      <c r="K56" s="6"/>
       <c r="L56" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15.75">
-      <c r="A57" s="7">
+      <c r="A57" s="4">
         <v>1</v>
       </c>
       <c r="B57" t="s">
@@ -3000,12 +3014,12 @@
       <c r="M57" t="s">
         <v>265</v>
       </c>
-      <c r="N57" s="18" t="s">
+      <c r="N57" s="12" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75">
-      <c r="A58" s="7">
+      <c r="A58" s="4">
         <v>1</v>
       </c>
       <c r="B58" t="s">
@@ -3023,12 +3037,12 @@
       <c r="M58" t="s">
         <v>266</v>
       </c>
-      <c r="N58" s="18" t="s">
+      <c r="N58" s="12" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="15.75">
-      <c r="A59" s="7">
+      <c r="A59" s="4">
         <v>1</v>
       </c>
       <c r="B59" t="s">
@@ -3049,12 +3063,12 @@
       <c r="M59" t="s">
         <v>267</v>
       </c>
-      <c r="N59" s="18" t="s">
+      <c r="N59" s="12" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15.75">
-      <c r="A60" s="7">
+      <c r="A60" s="4">
         <v>1</v>
       </c>
       <c r="B60" t="s">
@@ -3075,12 +3089,12 @@
       <c r="M60" t="s">
         <v>268</v>
       </c>
-      <c r="N60" s="18" t="s">
+      <c r="N60" s="12" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="15.75">
-      <c r="A61" s="7">
+      <c r="A61" s="4">
         <v>1</v>
       </c>
       <c r="B61" t="s">
@@ -3101,29 +3115,29 @@
       <c r="M61" t="s">
         <v>254</v>
       </c>
-      <c r="N61" s="18" t="s">
+      <c r="N61" s="12" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15.75">
-      <c r="A62" s="7">
+      <c r="A62" s="4">
         <v>1</v>
       </c>
       <c r="B62" t="s">
         <v>185</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" t="s">
         <v>185</v>
       </c>
       <c r="L62" t="s">
         <v>154</v>
       </c>
-      <c r="N62" s="18" t="s">
+      <c r="N62" s="12" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="15.75">
-      <c r="A63" s="7">
+      <c r="A63" s="4">
         <v>1</v>
       </c>
       <c r="B63" t="s">
@@ -3144,12 +3158,12 @@
       <c r="M63" t="s">
         <v>269</v>
       </c>
-      <c r="N63" s="18" t="s">
+      <c r="N63" s="12" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="15.75">
-      <c r="A64" s="7">
+      <c r="A64" s="4">
         <v>1</v>
       </c>
       <c r="B64" t="s">
@@ -3167,12 +3181,12 @@
       <c r="M64" t="s">
         <v>271</v>
       </c>
-      <c r="N64" s="18" t="s">
+      <c r="N64" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15.75">
-      <c r="A65" s="7">
+      <c r="A65" s="4">
         <v>1</v>
       </c>
       <c r="B65" t="s">
@@ -3189,7 +3203,7 @@
       </c>
     </row>
     <row r="66" spans="1:14" ht="15.75">
-      <c r="A66" s="7">
+      <c r="A66" s="4">
         <v>1</v>
       </c>
       <c r="B66" t="s">
@@ -3210,12 +3224,12 @@
       <c r="M66" t="s">
         <v>272</v>
       </c>
-      <c r="N66" s="18" t="s">
+      <c r="N66" s="12" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="15.75">
-      <c r="A67" s="7">
+      <c r="A67" s="4">
         <v>1</v>
       </c>
       <c r="B67" t="s">
@@ -3235,7 +3249,7 @@
       </c>
     </row>
     <row r="68" spans="1:14" ht="15.75">
-      <c r="A68" s="7">
+      <c r="A68" s="4">
         <v>1</v>
       </c>
       <c r="B68" t="s">
@@ -3258,7 +3272,7 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="15.75">
-      <c r="A69" s="7">
+      <c r="A69" s="4">
         <v>1</v>
       </c>
       <c r="B69" t="s">
@@ -3276,18 +3290,18 @@
       <c r="M69" t="s">
         <v>274</v>
       </c>
-      <c r="N69" s="18" t="s">
+      <c r="N69" s="12" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15.75">
-      <c r="A70" s="7">
+      <c r="A70" s="4">
         <v>1</v>
       </c>
       <c r="B70" t="s">
         <v>205</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" t="s">
         <v>237</v>
       </c>
       <c r="L70" t="s">
@@ -3295,7 +3309,7 @@
       </c>
     </row>
     <row r="71" spans="1:14" ht="15.75">
-      <c r="A71" s="7">
+      <c r="A71" s="4">
         <v>1</v>
       </c>
       <c r="B71" t="s">
@@ -3304,22 +3318,22 @@
       <c r="C71" t="s">
         <v>207</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E71" s="13"/>
+      <c r="E71" s="8"/>
       <c r="L71" t="s">
         <v>154</v>
       </c>
-      <c r="M71" s="13" t="s">
+      <c r="M71" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="N71" s="18" t="s">
+      <c r="N71" s="12" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15.75">
-      <c r="A72" s="7">
+      <c r="A72" s="4">
         <v>1</v>
       </c>
       <c r="B72" t="s">
@@ -3328,24 +3342,24 @@
       <c r="C72" t="s">
         <v>238</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="D72" t="s">
         <v>239</v>
       </c>
-      <c r="F72" s="17"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
       <c r="L72" t="s">
         <v>154</v>
       </c>
       <c r="M72" t="s">
         <v>277</v>
       </c>
-      <c r="N72" s="18" t="s">
+      <c r="N72" s="12" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="15.75">
-      <c r="A73" s="7">
+      <c r="A73" s="4">
         <v>1</v>
       </c>
       <c r="B73" t="s">
@@ -3365,7 +3379,7 @@
       </c>
     </row>
     <row r="74" spans="1:14" ht="15.75">
-      <c r="A74" s="7">
+      <c r="A74" s="4">
         <v>1</v>
       </c>
       <c r="B74" t="s">
@@ -3377,22 +3391,22 @@
       <c r="D74" t="s">
         <v>210</v>
       </c>
-      <c r="J74" s="13" t="s">
+      <c r="J74" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="K74" s="13"/>
+      <c r="K74" s="8"/>
       <c r="L74" t="s">
         <v>154</v>
       </c>
       <c r="M74" t="s">
         <v>279</v>
       </c>
-      <c r="N74" s="18" t="s">
+      <c r="N74" s="12" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="15.75">
-      <c r="A75" s="7">
+      <c r="A75" s="4">
         <v>1</v>
       </c>
       <c r="B75" t="s">
@@ -3415,7 +3429,7 @@
       </c>
     </row>
     <row r="76" spans="1:14" ht="15.75">
-      <c r="A76" s="7">
+      <c r="A76" s="4">
         <v>1</v>
       </c>
       <c r="B76" t="s">
@@ -3436,12 +3450,12 @@
       <c r="M76" t="s">
         <v>281</v>
       </c>
-      <c r="N76" s="18" t="s">
+      <c r="N76" s="12" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="15.75">
-      <c r="A77" s="7">
+      <c r="A77" s="4">
         <v>1</v>
       </c>
       <c r="B77" t="s">
@@ -3450,16 +3464,16 @@
       <c r="D77" t="s">
         <v>219</v>
       </c>
-      <c r="G77" s="14"/>
+      <c r="G77" s="9"/>
       <c r="L77" t="s">
         <v>154</v>
       </c>
-      <c r="M77" s="19" t="s">
+      <c r="M77" s="13" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="15.75">
-      <c r="A78" s="7">
+      <c r="A78" s="4">
         <v>1</v>
       </c>
       <c r="B78" t="s">
@@ -3482,7 +3496,7 @@
       </c>
     </row>
     <row r="79" spans="1:14" ht="15.75">
-      <c r="A79" s="7">
+      <c r="A79" s="4">
         <v>1</v>
       </c>
       <c r="B79" t="s">
@@ -3491,7 +3505,7 @@
       <c r="D79" t="s">
         <v>224</v>
       </c>
-      <c r="I79" s="13" t="s">
+      <c r="I79" s="8" t="s">
         <v>288</v>
       </c>
       <c r="J79" t="s">
@@ -3503,12 +3517,12 @@
       <c r="M79" t="s">
         <v>285</v>
       </c>
-      <c r="N79" s="18" t="s">
+      <c r="N79" s="12" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="15.75">
-      <c r="A80" s="7">
+      <c r="A80" s="4">
         <v>1</v>
       </c>
       <c r="B80" t="s">
@@ -3529,66 +3543,111 @@
       <c r="M80" t="s">
         <v>286</v>
       </c>
-      <c r="N80" s="18" t="s">
+      <c r="N80" s="12" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15.75">
-      <c r="A81" s="7"/>
+    <row r="81" spans="1:14">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>348</v>
+      </c>
+      <c r="C81" t="s">
+        <v>349</v>
+      </c>
+      <c r="D81" t="s">
+        <v>350</v>
+      </c>
+      <c r="J81" t="s">
+        <v>348</v>
+      </c>
+      <c r="L81" t="s">
+        <v>154</v>
+      </c>
+      <c r="N81" s="12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82" t="s">
+        <v>352</v>
+      </c>
+      <c r="D82" t="s">
+        <v>353</v>
+      </c>
+      <c r="G82" t="s">
+        <v>354</v>
+      </c>
+      <c r="J82" t="s">
+        <v>352</v>
+      </c>
+      <c r="L82" t="s">
+        <v>154</v>
+      </c>
+      <c r="N82" s="12" t="s">
+        <v>355</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B80 B83:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1"/>
-    <hyperlink ref="N7" r:id="rId2"/>
-    <hyperlink ref="N8" r:id="rId3"/>
-    <hyperlink ref="N9" r:id="rId4"/>
-    <hyperlink ref="N10" r:id="rId5"/>
-    <hyperlink ref="N11" r:id="rId6"/>
-    <hyperlink ref="N26" r:id="rId7"/>
-    <hyperlink ref="N27" r:id="rId8"/>
-    <hyperlink ref="N28" r:id="rId9"/>
-    <hyperlink ref="N35" r:id="rId10"/>
-    <hyperlink ref="N33" r:id="rId11"/>
-    <hyperlink ref="N36" r:id="rId12"/>
-    <hyperlink ref="N37" r:id="rId13"/>
-    <hyperlink ref="N29" r:id="rId14"/>
-    <hyperlink ref="N30" r:id="rId15"/>
-    <hyperlink ref="N31" r:id="rId16"/>
-    <hyperlink ref="N32" r:id="rId17"/>
-    <hyperlink ref="N34" r:id="rId18"/>
-    <hyperlink ref="N38" r:id="rId19"/>
-    <hyperlink ref="N39" r:id="rId20"/>
-    <hyperlink ref="N40" r:id="rId21"/>
-    <hyperlink ref="N41" r:id="rId22"/>
-    <hyperlink ref="N42" r:id="rId23"/>
-    <hyperlink ref="N47" r:id="rId24"/>
-    <hyperlink ref="N49" r:id="rId25"/>
-    <hyperlink ref="N50" r:id="rId26"/>
-    <hyperlink ref="N51" r:id="rId27"/>
-    <hyperlink ref="N52" r:id="rId28"/>
-    <hyperlink ref="N53" r:id="rId29"/>
-    <hyperlink ref="N57" r:id="rId30"/>
-    <hyperlink ref="N58" r:id="rId31"/>
-    <hyperlink ref="N59" r:id="rId32"/>
-    <hyperlink ref="N60" r:id="rId33"/>
-    <hyperlink ref="N61" r:id="rId34"/>
-    <hyperlink ref="N62" r:id="rId35"/>
-    <hyperlink ref="N63" r:id="rId36"/>
-    <hyperlink ref="N64" r:id="rId37"/>
-    <hyperlink ref="N66" r:id="rId38"/>
-    <hyperlink ref="N69" r:id="rId39"/>
-    <hyperlink ref="N71" r:id="rId40"/>
-    <hyperlink ref="N72" r:id="rId41"/>
-    <hyperlink ref="N74" r:id="rId42"/>
-    <hyperlink ref="N76" r:id="rId43"/>
-    <hyperlink ref="M77" r:id="rId44"/>
-    <hyperlink ref="N79" r:id="rId45"/>
-    <hyperlink ref="N80" r:id="rId46"/>
+    <hyperlink ref="N6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="N10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="N11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="N26" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N27" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="N28" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="N35" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="N33" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N36" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="N37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="N29" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="N30" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="N31" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="N32" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="N34" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="N38" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="N39" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="N40" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="N41" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="N42" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="N47" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="N49" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="N50" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="N51" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="N52" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="N53" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="N57" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="N58" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="N59" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="N60" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="N61" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="N62" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="N63" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="N64" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="N66" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="N69" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="N71" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="N72" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="N74" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="N76" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="M77" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="N79" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="N80" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="N81" r:id="rId47" xr:uid="{90C10041-31F0-45A2-9F4B-253E03F8DAF5}"/>
+    <hyperlink ref="N82" r:id="rId48" xr:uid="{3080F2EA-3A4E-49FE-9E53-7C30884F0859}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId47"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: slug in funders
</commit_message>
<xml_diff>
--- a/data/excel/funders.xlsx
+++ b/data/excel/funders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\metadatové modely\nr-github\nr-taxonomies\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4746160-155B-4630-8D64-BDDABCD34933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894AD992-D20B-4365-A1A9-AD54F2F26B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33255" yWindow="690" windowWidth="21600" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1755" windowWidth="25680" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nr" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="357">
   <si>
     <t>code</t>
   </si>
@@ -1096,6 +1096,9 @@
   </si>
   <si>
     <t>https://ror.org/037nx0e70</t>
+  </si>
+  <si>
+    <t>UPCE-f</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1511,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15"/>
@@ -3552,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="C81" t="s">
         <v>349</v>

</xml_diff>

<commit_message>
fixed alias for masaryk university
</commit_message>
<xml_diff>
--- a/data/excel/funders.xlsx
+++ b/data/excel/funders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vackovab\Documents\nr-taxonomies\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6858283-3737-4F6B-895F-4720F76BB74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE552091-8A88-4B75-9754-516273532199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nr" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="362">
   <si>
     <t>code</t>
   </si>
@@ -1111,6 +1111,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://ror.org/02j46qs45 </t>
+  </si>
+  <si>
+    <t>MU</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1199,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1225,7 +1228,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hypertextový odkaz" xfId="2" builtinId="8"/>
@@ -1521,27 +1523,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="M83" sqref="M83"/>
+      <selection pane="bottomLeft" activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" customWidth="1"/>
-    <col min="13" max="13" width="37.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6">
+    <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1563,7 @@
       <c r="K1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="15.6">
+    <row r="2" spans="1:14" ht="15.75">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1581,7 +1583,7 @@
       <c r="K2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="15.6">
+    <row r="3" spans="1:14" ht="15.75">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1595,7 +1597,7 @@
       <c r="K3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="15.6">
+    <row r="5" spans="1:14" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1639,7 +1641,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.6">
+    <row r="6" spans="1:14" ht="15.75">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1673,7 +1675,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.6">
+    <row r="7" spans="1:14" ht="15.75">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1703,7 +1705,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.6">
+    <row r="8" spans="1:14" ht="15.75">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.6">
+    <row r="9" spans="1:14" ht="15.75">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1765,7 +1767,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.6">
+    <row r="10" spans="1:14" ht="15.75">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1795,7 +1797,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.6">
+    <row r="11" spans="1:14" ht="15.75">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.6">
+    <row r="12" spans="1:14" ht="15.75">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1854,7 +1856,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:14" ht="15.6">
+    <row r="13" spans="1:14" ht="15.75">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1879,7 +1881,7 @@
       </c>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:14" ht="15.6">
+    <row r="14" spans="1:14" ht="15.75">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1904,7 +1906,7 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:14" ht="15.6">
+    <row r="15" spans="1:14" ht="15.75">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1929,7 +1931,7 @@
       </c>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:14" ht="15.6">
+    <row r="16" spans="1:14" ht="15.75">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1954,7 +1956,7 @@
       </c>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:14" ht="15.6">
+    <row r="17" spans="1:14" ht="15.75">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1979,7 +1981,7 @@
       </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:14" ht="15.6">
+    <row r="18" spans="1:14" ht="15.75">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -2004,7 +2006,7 @@
       </c>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="15.6">
+    <row r="19" spans="1:14" ht="15.75">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -2029,7 +2031,7 @@
       </c>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:14" ht="15.6">
+    <row r="20" spans="1:14" ht="15.75">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -2054,7 +2056,7 @@
       </c>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:14" ht="15.6">
+    <row r="21" spans="1:14" ht="15.75">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -2079,7 +2081,7 @@
       </c>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="15.6">
+    <row r="22" spans="1:14" ht="15.75">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -2104,7 +2106,7 @@
       </c>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:14" ht="15.6">
+    <row r="23" spans="1:14" ht="15.75">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -2129,7 +2131,7 @@
       </c>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:14" ht="15.6">
+    <row r="24" spans="1:14" ht="15.75">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -2154,7 +2156,7 @@
       </c>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="15.6">
+    <row r="25" spans="1:14" ht="15.75">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -2179,7 +2181,7 @@
       </c>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:14" ht="15.6">
+    <row r="26" spans="1:14" ht="15.75">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -2211,7 +2213,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.6">
+    <row r="27" spans="1:14" ht="15.75">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.6">
+    <row r="28" spans="1:14" ht="15.75">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -2273,7 +2275,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.6">
+    <row r="29" spans="1:14" ht="15.75">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -2303,7 +2305,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.6">
+    <row r="30" spans="1:14" ht="15.75">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -2335,7 +2337,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.6">
+    <row r="31" spans="1:14" ht="15.75">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -2367,7 +2369,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.6">
+    <row r="32" spans="1:14" ht="15.75">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -2399,7 +2401,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.6">
+    <row r="33" spans="1:14" ht="15.75">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.6">
+    <row r="34" spans="1:14" ht="15.75">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.6">
+    <row r="35" spans="1:14" ht="15.75">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -2493,7 +2495,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.6">
+    <row r="36" spans="1:14" ht="15.75">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -2525,7 +2527,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.6">
+    <row r="37" spans="1:14" ht="15.75">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -2557,7 +2559,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.6">
+    <row r="38" spans="1:14" ht="15.75">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -2589,7 +2591,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.6">
+    <row r="39" spans="1:14" ht="15.75">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -2619,7 +2621,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.6">
+    <row r="40" spans="1:14" ht="15.75">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -2649,7 +2651,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.6">
+    <row r="41" spans="1:14" ht="15.75">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2673,7 +2675,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.6">
+    <row r="42" spans="1:14" ht="15.75">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -2702,7 +2704,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.6">
+    <row r="43" spans="1:14" ht="15.75">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -2721,7 +2723,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.6">
+    <row r="44" spans="1:14" ht="15.75">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -2740,7 +2742,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15.6">
+    <row r="45" spans="1:14" ht="15.75">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -2761,7 +2763,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15.6">
+    <row r="46" spans="1:14" ht="15.75">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15.6">
+    <row r="47" spans="1:14" ht="15.75">
       <c r="A47" s="4">
         <v>1</v>
       </c>
@@ -2809,7 +2811,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.6">
+    <row r="48" spans="1:14" ht="15.75">
       <c r="A48" s="4">
         <v>1</v>
       </c>
@@ -2833,7 +2835,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15.6">
+    <row r="49" spans="1:14" ht="15.75">
       <c r="A49" s="4">
         <v>1</v>
       </c>
@@ -2857,7 +2859,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15.6">
+    <row r="50" spans="1:14" ht="15.75">
       <c r="A50" s="4">
         <v>1</v>
       </c>
@@ -2884,7 +2886,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15.6">
+    <row r="51" spans="1:14" ht="15.75">
       <c r="A51" s="4">
         <v>1</v>
       </c>
@@ -2911,7 +2913,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15.6">
+    <row r="52" spans="1:14" ht="15.75">
       <c r="A52" s="4">
         <v>1</v>
       </c>
@@ -2938,7 +2940,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15.6">
+    <row r="53" spans="1:14" ht="15.75">
       <c r="A53" s="4">
         <v>1</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15.6">
+    <row r="54" spans="1:14" ht="15.75">
       <c r="A54" s="4">
         <v>1</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15.6">
+    <row r="55" spans="1:14" ht="15.75">
       <c r="A55" s="4">
         <v>1</v>
       </c>
@@ -2996,7 +2998,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15.6">
+    <row r="56" spans="1:14" ht="15.75">
       <c r="A56" s="4">
         <v>1</v>
       </c>
@@ -3014,7 +3016,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15.6">
+    <row r="57" spans="1:14" ht="15.75">
       <c r="A57" s="4">
         <v>1</v>
       </c>
@@ -3034,7 +3036,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15.6">
+    <row r="58" spans="1:14" ht="15.75">
       <c r="A58" s="4">
         <v>1</v>
       </c>
@@ -3057,7 +3059,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15.6">
+    <row r="59" spans="1:14" ht="15.75">
       <c r="A59" s="4">
         <v>1</v>
       </c>
@@ -3083,7 +3085,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15.6">
+    <row r="60" spans="1:14" ht="15.75">
       <c r="A60" s="4">
         <v>1</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15.6">
+    <row r="61" spans="1:14" ht="15.75">
       <c r="A61" s="4">
         <v>1</v>
       </c>
@@ -3135,7 +3137,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15.6">
+    <row r="62" spans="1:14" ht="15.75">
       <c r="A62" s="4">
         <v>1</v>
       </c>
@@ -3152,7 +3154,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15.6">
+    <row r="63" spans="1:14" ht="15.75">
       <c r="A63" s="4">
         <v>1</v>
       </c>
@@ -3178,7 +3180,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15.6">
+    <row r="64" spans="1:14" ht="15.75">
       <c r="A64" s="4">
         <v>1</v>
       </c>
@@ -3201,7 +3203,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15.6">
+    <row r="65" spans="1:14" ht="15.75">
       <c r="A65" s="4">
         <v>1</v>
       </c>
@@ -3218,7 +3220,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15.6">
+    <row r="66" spans="1:14" ht="15.75">
       <c r="A66" s="4">
         <v>1</v>
       </c>
@@ -3244,7 +3246,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15.6">
+    <row r="67" spans="1:14" ht="15.75">
       <c r="A67" s="4">
         <v>1</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15.6">
+    <row r="68" spans="1:14" ht="15.75">
       <c r="A68" s="4">
         <v>1</v>
       </c>
@@ -3287,7 +3289,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15.6">
+    <row r="69" spans="1:14" ht="15.75">
       <c r="A69" s="4">
         <v>1</v>
       </c>
@@ -3310,7 +3312,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15.6">
+    <row r="70" spans="1:14" ht="15.75">
       <c r="A70" s="4">
         <v>1</v>
       </c>
@@ -3324,7 +3326,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15.6">
+    <row r="71" spans="1:14" ht="15.75">
       <c r="A71" s="4">
         <v>1</v>
       </c>
@@ -3348,7 +3350,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15.6">
+    <row r="72" spans="1:14" ht="15.75">
       <c r="A72" s="4">
         <v>1</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15.6">
+    <row r="73" spans="1:14" ht="15.75">
       <c r="A73" s="4">
         <v>1</v>
       </c>
@@ -3394,7 +3396,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15.6">
+    <row r="74" spans="1:14" ht="15.75">
       <c r="A74" s="4">
         <v>1</v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15.6">
+    <row r="75" spans="1:14" ht="15.75">
       <c r="A75" s="4">
         <v>1</v>
       </c>
@@ -3444,7 +3446,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15.6">
+    <row r="76" spans="1:14" ht="15.75">
       <c r="A76" s="4">
         <v>1</v>
       </c>
@@ -3470,7 +3472,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15.6">
+    <row r="77" spans="1:14" ht="15.75">
       <c r="A77" s="4">
         <v>1</v>
       </c>
@@ -3488,7 +3490,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15.6">
+    <row r="78" spans="1:14" ht="15.75">
       <c r="A78" s="4">
         <v>1</v>
       </c>
@@ -3511,7 +3513,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15.6">
+    <row r="79" spans="1:14" ht="15.75">
       <c r="A79" s="4">
         <v>1</v>
       </c>
@@ -3537,7 +3539,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15.6">
+    <row r="80" spans="1:14" ht="15.75">
       <c r="A80" s="4">
         <v>1</v>
       </c>
@@ -3609,8 +3611,8 @@
         <v>355</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15.6">
-      <c r="A83" s="14">
+    <row r="83" spans="1:14" ht="15.75">
+      <c r="A83" s="4">
         <v>1</v>
       </c>
       <c r="B83" t="s">
@@ -3623,6 +3625,9 @@
         <v>359</v>
       </c>
       <c r="J83" t="s">
+        <v>361</v>
+      </c>
+      <c r="K83" t="s">
         <v>357</v>
       </c>
       <c r="L83" t="s">

</xml_diff>

<commit_message>
new funder ga ju
grant agency of uni of south bohemia
</commit_message>
<xml_diff>
--- a/data/excel/funders.xlsx
+++ b/data/excel/funders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vackovab\Documents\nr-taxonomies\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995AD5A1-6666-4584-82F6-A44EA0D9703F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1497BF-4B8B-4609-BFAE-AFE974F59964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nr" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="374">
   <si>
     <t>code</t>
   </si>
@@ -1138,6 +1138,18 @@
   </si>
   <si>
     <t>https://ror.org/0472cxd90</t>
+  </si>
+  <si>
+    <t>GA-JU</t>
+  </si>
+  <si>
+    <t>Grantová agentura Jihočeské univerzity</t>
+  </si>
+  <si>
+    <t>Grant Agency of University of South Bohemia</t>
+  </si>
+  <si>
+    <t>GA JU</t>
   </si>
 </sst>
 </file>
@@ -1546,12 +1558,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15"/>
@@ -3686,7 +3698,7 @@
       </c>
     </row>
     <row r="85" spans="1:14" ht="15.75">
-      <c r="A85" s="14">
+      <c r="A85" s="4">
         <v>1</v>
       </c>
       <c r="B85" t="s">
@@ -3706,6 +3718,26 @@
       </c>
       <c r="N85" s="12" t="s">
         <v>369</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="15.75">
+      <c r="A86" s="14">
+        <v>1</v>
+      </c>
+      <c r="B86" t="s">
+        <v>370</v>
+      </c>
+      <c r="C86" t="s">
+        <v>371</v>
+      </c>
+      <c r="D86" t="s">
+        <v>372</v>
+      </c>
+      <c r="J86" t="s">
+        <v>373</v>
+      </c>
+      <c r="L86" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>